<commit_message>
Small update to Template file and gitignore
Update template file with shorter names, bigger series column, and Small sheet as default. remove output.csv from .gitignore as program works better if it's there.
</commit_message>
<xml_diff>
--- a/templates/TemplateAll.xlsx
+++ b/templates/TemplateAll.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D9C4E7-EFE5-4940-8F88-52933AA0C173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0FAB3F-9CE8-4F8D-B8FB-BFF4EB8620E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BECE5613-4CE6-4BB7-8FF1-F4E60925457F}"/>
+    <workbookView xWindow="-27825" yWindow="1515" windowWidth="16485" windowHeight="13440" xr2:uid="{BECE5613-4CE6-4BB7-8FF1-F4E60925457F}"/>
   </bookViews>
   <sheets>
-    <sheet name="iRacingCalendarTemplateSmall" sheetId="2" r:id="rId1"/>
-    <sheet name="iRacingCalendarTemplateLarge" sheetId="3" r:id="rId2"/>
+    <sheet name="Small" sheetId="2" r:id="rId1"/>
+    <sheet name="Large" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -950,8 +950,8 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1008,7 @@
       <c r="K3" s="29"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:26" ht="36.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
@@ -1413,7 +1413,8 @@
       <formula>$L5="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.2" right="0.2" top="0.4" bottom="0.4" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.2" right="0.2" top="0.2" bottom="0.2" header="0" footer="0"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
@@ -1423,7 +1424,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:EV18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="EF6" sqref="EF6"/>
     </sheetView>
   </sheetViews>

</xml_diff>